<commit_message>
Observaciones corregidas del Reporte BoletaVentaGNSUnnaEnergiaLimasGas
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletaVentaGnsUnnaEnergiaLimagas.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletaVentaGnsUnnaEnergiaLimagas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27816"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza7\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7C26B8-9B19-4C71-80FA-4270229DECB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578E3CC3-3BA1-4B1A-A722-C0E29F3955C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F6C72EAA-4D7F-408A-95FB-FC029C6B19CD}"/>
+    <workbookView xWindow="3432" yWindow="900" windowWidth="17280" windowHeight="8964" xr2:uid="{F6C72EAA-4D7F-408A-95FB-FC029C6B19CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
     <numFmt numFmtId="171" formatCode="0.0000"/>
     <numFmt numFmtId="172" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,14 +234,6 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -625,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -639,227 +631,230 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -937,6 +932,56 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>701303</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F812F57B-2E0C-4C63-9E5F-2B967843CEB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1165861" y="5829300"/>
+          <a:ext cx="1318522" cy="632460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1241,101 +1286,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9856E028-0575-4EE5-B24C-B009DA133258}">
-  <dimension ref="B3:N32"/>
+  <dimension ref="B3:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B3" sqref="B3:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.44140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.42578125" style="2"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="14" width="11.44140625" style="2"/>
+    <col min="15" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="76" t="s">
+    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-    </row>
-    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+    </row>
+    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
       <c r="I5" s="5"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="78" t="s">
+    <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="78" t="s">
+      <c r="E7" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="78" t="s">
+      <c r="F7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="78" t="s">
+      <c r="G7" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="78" t="s">
+      <c r="I7" s="74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="78"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-    </row>
-    <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="74"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+    </row>
+    <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
         <v>11</v>
       </c>
@@ -1361,7 +1406,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
@@ -1371,14 +1416,14 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="73" t="s">
+    <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
       <c r="G11" s="15" t="s">
         <v>20</v>
       </c>
@@ -1389,7 +1434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -1399,7 +1444,7 @@
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
@@ -1413,11 +1458,11 @@
       </c>
       <c r="I13" s="23"/>
     </row>
-    <row r="14" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="25" t="s">
         <v>23</v>
       </c>
@@ -1431,7 +1476,7 @@
       </c>
       <c r="I15" s="30"/>
     </row>
-    <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -1441,7 +1486,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="32"/>
     </row>
-    <row r="17" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="25" t="s">
         <v>25</v>
       </c>
@@ -1455,7 +1500,7 @@
       </c>
       <c r="I17" s="37"/>
     </row>
-    <row r="18" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="38" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1516,7 @@
       </c>
       <c r="I18" s="44"/>
     </row>
-    <row r="19" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="45" t="s">
         <v>30</v>
       </c>
@@ -1487,7 +1532,7 @@
       </c>
       <c r="I19" s="51"/>
     </row>
-    <row r="20" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="52" t="s">
         <v>33</v>
       </c>
@@ -1503,7 +1548,7 @@
       </c>
       <c r="I20" s="44"/>
     </row>
-    <row r="21" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="58"/>
       <c r="C21" s="58"/>
       <c r="D21" s="58"/>
@@ -1513,7 +1558,7 @@
       <c r="H21" s="59"/>
       <c r="I21" s="31"/>
     </row>
-    <row r="22" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="60" t="s">
         <v>36</v>
       </c>
@@ -1527,7 +1572,7 @@
       </c>
       <c r="I22" s="63"/>
     </row>
-    <row r="23" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="64" t="s">
         <v>38</v>
       </c>
@@ -1541,7 +1586,7 @@
       </c>
       <c r="I23" s="31"/>
     </row>
-    <row r="24" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="25" t="s">
         <v>40</v>
       </c>
@@ -1555,7 +1600,7 @@
       </c>
       <c r="I24" s="31"/>
     </row>
-    <row r="25" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="58"/>
       <c r="C25" s="58"/>
       <c r="D25" s="58"/>
@@ -1565,7 +1610,7 @@
       <c r="H25" s="69"/>
       <c r="I25" s="31"/>
     </row>
-    <row r="26" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="63"/>
       <c r="C26" s="63"/>
       <c r="D26" s="63"/>
@@ -1575,7 +1620,7 @@
       <c r="H26" s="63"/>
       <c r="I26" s="63"/>
     </row>
-    <row r="27" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="70" t="s">
         <v>42</v>
       </c>
@@ -1587,39 +1632,39 @@
       <c r="H27" s="31"/>
       <c r="I27" s="31"/>
     </row>
-    <row r="28" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="74" t="s">
+    <row r="28" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="74"/>
-    </row>
-    <row r="29" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-    </row>
-    <row r="30" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-    </row>
-    <row r="31" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
+    </row>
+    <row r="29" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78"/>
+    </row>
+    <row r="30" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
+    </row>
+    <row r="31" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="31"/>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
@@ -1629,22 +1674,30 @@
       <c r="H31" s="31"/>
       <c r="I31" s="31"/>
     </row>
-    <row r="32" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="31"/>
-      <c r="C32" s="75" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="75"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="79"/>
       <c r="E32" s="31"/>
-      <c r="F32" s="75" t="s">
-        <v>45</v>
-      </c>
-      <c r="G32" s="75"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="79"/>
       <c r="H32" s="31"/>
       <c r="I32" s="31"/>
     </row>
+    <row r="35" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="76"/>
+      <c r="F35" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="76"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:G35"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B28:I30"/>
     <mergeCell ref="C32:D32"/>

</xml_diff>